<commit_message>
add and remove debugged
</commit_message>
<xml_diff>
--- a/Documents/Sprint Plan/SprintPlan.xlsx
+++ b/Documents/Sprint Plan/SprintPlan.xlsx
@@ -143,9 +143,6 @@
     <t>Sunday, November 27,2016</t>
   </si>
   <si>
-    <t>Sunday, December 4,2016</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
@@ -188,18 +185,9 @@
     <t>Implementing the run simulation</t>
   </si>
   <si>
-    <t>Friday,December,23, 2016</t>
-  </si>
-  <si>
-    <t>Monday, January 9, 2017</t>
-  </si>
-  <si>
     <t>Sunday, January 15,2017</t>
   </si>
   <si>
-    <t>Monday, December 5, 2016</t>
-  </si>
-  <si>
     <t>Implementing there Information Panel</t>
   </si>
   <si>
@@ -207,6 +195,18 @@
   </si>
   <si>
     <t>Fertilizer Selection</t>
+  </si>
+  <si>
+    <t>Sunday, December 11,2016</t>
+  </si>
+  <si>
+    <t>Monday, December 12, 2016</t>
+  </si>
+  <si>
+    <t>Wedneesday, January 11, 2017</t>
+  </si>
+  <si>
+    <t>Tuesday,January,10, 2016</t>
   </si>
 </sst>
 </file>
@@ -762,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -989,10 +989,10 @@
         <v>165</v>
       </c>
       <c r="G7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="5"/>
@@ -1020,7 +1020,7 @@
         <v>101</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>21</v>
@@ -1037,7 +1037,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -1064,7 +1064,7 @@
         <v>102</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -1106,7 +1106,7 @@
         <v>103</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -1123,7 +1123,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -1167,7 +1167,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -1194,7 +1194,7 @@
         <v>105</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>10</v>
@@ -1211,7 +1211,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -1255,7 +1255,7 @@
         <v>36</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="5"/>
@@ -1300,7 +1300,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -1344,7 +1344,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -1371,7 +1371,7 @@
         <v>203</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>9</v>
@@ -1388,7 +1388,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -1432,7 +1432,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
@@ -1476,7 +1476,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -1503,7 +1503,7 @@
         <v>206</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>9</v>
@@ -1520,7 +1520,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
@@ -1564,7 +1564,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
@@ -1608,7 +1608,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -1635,7 +1635,7 @@
         <v>209</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>9</v>
@@ -1652,7 +1652,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -1679,7 +1679,7 @@
         <v>210</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>10</v>
@@ -1696,7 +1696,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -1737,10 +1737,10 @@
         <v>190</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="5"/>
@@ -1768,7 +1768,7 @@
         <v>301</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>9</v>
@@ -1785,7 +1785,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -1829,7 +1829,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -1873,7 +1873,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -1917,7 +1917,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -1944,7 +1944,7 @@
         <v>305</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>9</v>
@@ -1961,7 +1961,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -1988,7 +1988,7 @@
         <v>306</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>9</v>
@@ -2005,7 +2005,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -2032,7 +2032,7 @@
         <v>307</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>10</v>
@@ -2049,7 +2049,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -2089,10 +2089,10 @@
         <v>165</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="5"/>
@@ -2137,7 +2137,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -2181,7 +2181,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -2208,7 +2208,7 @@
         <v>403</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>10</v>
@@ -2225,7 +2225,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>

</xml_diff>